<commit_message>
Display-user komment_szerzo_id javítva, placeholder img hozzáadva a display-users-hez.
</commit_message>
<xml_diff>
--- a/docs/Táblázatok_kifejtése.xlsx
+++ b/docs/Táblázatok_kifejtése.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="100">
   <si>
     <t xml:space="preserve">Név</t>
   </si>
@@ -148,10 +148,11 @@
 Lehet null, külső kulcs.</t>
   </si>
   <si>
-    <t xml:space="preserve">poszt_felh_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poszt tulajdonos azonosító</t>
+    <t xml:space="preserve">poszt_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A kapcsolódó poszt azonosítója.
+Nem lehet null, külső kulcs.</t>
   </si>
   <si>
     <t xml:space="preserve">csatl_dat</t>
@@ -169,11 +170,14 @@
 Lehet null, külső kulcs.</t>
   </si>
   <si>
-    <t xml:space="preserve">poszt_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A kapcsolódó poszt azonosítója.
-Nem lehet null, külső kulcs.</t>
+    <t xml:space="preserve">szoveg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARCHAR(1000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A komment szövege.
+Nem lehet null.</t>
   </si>
   <si>
     <t xml:space="preserve">szul_dat</t>
@@ -183,18 +187,18 @@
 Nem lehet null.</t>
   </si>
   <si>
-    <t xml:space="preserve">szoveg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VARCHAR(1000)</t>
-  </si>
-  <si>
     <t xml:space="preserve">A poszt szövege.
 Nem lehet null.</t>
   </si>
   <si>
-    <t xml:space="preserve">A komment szövege.
-Nem lehet null.</t>
+    <t xml:space="preserve">ertekeles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERTEKELES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A komment értékelése.
+Nem lehet null</t>
   </si>
   <si>
     <t xml:space="preserve">munka_iskola</t>
@@ -208,18 +212,18 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">ertekeles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERTEKELES</t>
-  </si>
-  <si>
     <t xml:space="preserve">A poszt értékelése (Like-ok, dislike-ok.)
 Nem lehet null.</t>
   </si>
   <si>
-    <t xml:space="preserve">A komment értékelése.
-Nem lehet null</t>
+    <t xml:space="preserve">isPublic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUMBER(1, 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A komment publicitása.
+Nem lehet null.</t>
   </si>
   <si>
     <t xml:space="preserve">picture</t>
@@ -232,17 +236,7 @@
 Lehet null.</t>
   </si>
   <si>
-    <t xml:space="preserve">isPublic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUMBER(1, 0)</t>
-  </si>
-  <si>
     <t xml:space="preserve">A poszt publicitása. (Publikus-e, vagy nem.)
-Nem lehet null.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A komment publicitása.
 Nem lehet null.</t>
   </si>
   <si>
@@ -393,6 +387,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -415,6 +410,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -580,8 +576,8 @@
   </sheetPr>
   <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O12" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q12" activeCellId="0" sqref="Q12:W14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5:O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -796,7 +792,7 @@
       <c r="N5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -823,108 +819,102 @@
         <v>42</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="M7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="M7" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="N7" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="M8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="M8" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="N8" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="J9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K9" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>63</v>
-      </c>
+      <c r="M9" s="0"/>
+      <c r="N9" s="0"/>
+      <c r="O9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" s="3" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -991,7 +981,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>40</v>
@@ -1000,7 +990,7 @@
         <v>4</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>40</v>
@@ -1009,34 +999,34 @@
         <v>4</v>
       </c>
       <c r="K13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q13" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="R13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="S13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="N13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q13" s="4" t="s">
+      <c r="U13" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="R13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="S13" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="U13" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="V13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1047,16 +1037,16 @@
         <v>18</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>6</v>
@@ -1065,45 +1055,45 @@
         <v>4</v>
       </c>
       <c r="K14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q14" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="R14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="S14" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="N14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="O14" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q14" s="4" t="s">
+      <c r="U14" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="R14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="S14" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="U14" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="V14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>6</v>
@@ -1112,18 +1102,18 @@
         <v>4</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>17</v>
@@ -1132,7 +1122,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I16" s="0"/>
       <c r="J16" s="0"/>
@@ -1140,22 +1130,22 @@
     </row>
     <row r="17" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="I17" s="0"/>
       <c r="J17" s="0"/>
@@ -1194,69 +1184,69 @@
         <v>25</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="F21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E22" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E23" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E24" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>